<commit_message>
close. use hash tables.
</commit_message>
<xml_diff>
--- a/nursing/data/nursing.xlsx
+++ b/nursing/data/nursing.xlsx
@@ -6,7 +6,9 @@
     <workbookView activeTab="0" firstSheet="0" windowHeight="13125" windowWidth="13125" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet 1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="week" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="provider" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="state" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
 </workbook>
 </file>
@@ -42,8 +44,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="14" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -349,12 +352,329 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
-  <dimension ref="A1"/>
+  <dimension ref="A1:A32"/>
   <sheetViews>
     <sheetView showGridLines="1" showRowColHeaders="1" tabSelected="1" workbookViewId="0" zoomScale="100"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="8.43" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1">
+        <v>43975</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1">
+        <v>43982</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1">
+        <v>43989</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1">
+        <v>43996</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1">
+        <v>44003</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1">
+        <v>44010</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1">
+        <v>44017</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1">
+        <v>44024</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1">
+        <v>44031</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1">
+        <v>44038</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1">
+        <v>44045</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1">
+        <v>44052</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="1">
+        <v>44059</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="1">
+        <v>44066</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="1">
+        <v>44073</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="1">
+        <v>44080</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="1">
+        <v>44087</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="1">
+        <v>44094</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="1">
+        <v>44101</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="1">
+        <v>44108</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="1">
+        <v>44115</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="1">
+        <v>44122</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="1">
+        <v>44129</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="1">
+        <v>44136</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="1">
+        <v>44143</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="1">
+        <v>44150</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="1">
+        <v>44157</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="1">
+        <v>44164</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="1">
+        <v>44171</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="1">
+        <v>44178</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="1">
+        <v>44185</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="1">
+        <v>44192</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions gridLines="1" gridLinesSet="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
+  <dimension ref="A1:A17"/>
+  <sheetViews>
+    <sheetView showGridLines="1" showRowColHeaders="1" tabSelected="0" workbookViewId="0" zoomScale="100"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8.43" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>015009</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>015010</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>015012</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>015014</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>015015</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>015016</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>015019</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>015023</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>015024</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>015027</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>015028</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>015031</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>015032</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>015034</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>015035</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>015037</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>015040</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions gridLines="1" gridLinesSet="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView showGridLines="1" showRowColHeaders="1" tabSelected="0" workbookViewId="0" zoomScale="100"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8.43" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>AL</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
   <printOptions gridLines="1" gridLinesSet="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>